<commit_message>
Edit some fields of tables in excel file.
</commit_message>
<xml_diff>
--- a/Document/Final-Design-Database.xlsx
+++ b/Document/Final-Design-Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PTIT-BookStore-Website-Project\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFFD606-BF98-4AA4-9C08-30FC0008B3F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4614B1B9-DBE0-4526-B86B-6BE9DA657EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QUICKLOOK" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,10 @@
     <sheet name="AUTHOR" sheetId="15" r:id="rId3"/>
     <sheet name="CATEGORY" sheetId="14" r:id="rId4"/>
     <sheet name="BOOK" sheetId="2" r:id="rId5"/>
-    <sheet name="CART" sheetId="17" r:id="rId6"/>
-    <sheet name="PROMOTION" sheetId="20" r:id="rId7"/>
-    <sheet name="USERACCOUNT" sheetId="18" r:id="rId8"/>
-    <sheet name="DELIVERYINFORMATION" sheetId="24" r:id="rId9"/>
+    <sheet name="PROMOTION" sheetId="20" r:id="rId6"/>
+    <sheet name="USERACCOUNT" sheetId="18" r:id="rId7"/>
+    <sheet name="DELIVERYINFORMATION" sheetId="24" r:id="rId8"/>
+    <sheet name="CART" sheetId="17" r:id="rId9"/>
     <sheet name="MASTERROLE" sheetId="26" r:id="rId10"/>
     <sheet name="STAFFACCOUNT" sheetId="23" r:id="rId11"/>
     <sheet name="ORDER" sheetId="21" r:id="rId12"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="167">
   <si>
     <t>SatisfyProduct</t>
   </si>
@@ -451,9 +451,6 @@
     <t>char(10)</t>
   </si>
   <si>
-    <t>varchar(100)</t>
-  </si>
-  <si>
     <t>0 là đang làm, 1 là đã nghỉ</t>
   </si>
   <si>
@@ -539,6 +536,9 @@
   </si>
   <si>
     <t>Ý tưởng thông minh</t>
+  </si>
+  <si>
+    <t>Phone</t>
   </si>
 </sst>
 </file>
@@ -736,10 +736,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1031,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,7 +1070,7 @@
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J1" s="2"/>
       <c r="L1" s="2"/>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="J2" s="2"/>
       <c r="L2" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -1314,7 +1314,7 @@
     </row>
     <row r="12" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B12" s="2"/>
       <c r="D12" s="2"/>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="4" t="s">
@@ -1466,7 +1466,7 @@
     </row>
     <row r="19" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="5" t="s">
@@ -1510,7 +1510,7 @@
       <c r="D22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H22" s="2"/>
       <c r="J22" s="2"/>
@@ -1618,7 +1618,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1674,10 +1674,10 @@
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1688,14 +1688,14 @@
         <v>65</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
         <v>44</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1711,7 +1711,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>129</v>
@@ -1787,7 +1787,7 @@
         <v>47</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1825,7 +1825,7 @@
         <v>44</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1843,7 +1843,7 @@
         <v>47</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1851,7 +1851,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>62</v>
+        <v>166</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>136</v>
@@ -1861,7 +1861,7 @@
         <v>47</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1879,7 +1879,7 @@
         <v>83</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1915,7 +1915,7 @@
         <v>44</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1926,14 +1926,14 @@
         <v>22</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1959,7 +1959,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>49</v>
@@ -1969,7 +1969,7 @@
         <v>83</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1984,7 +1984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE317E5-52A0-4284-95B8-DCBD3874C7B7}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -2041,7 +2041,7 @@
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>126</v>
@@ -2052,7 +2052,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>40</v>
@@ -2170,7 +2170,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2238,8 +2238,11 @@
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="C4" s="10" t="s">
+        <v>50</v>
+      </c>
       <c r="D4" s="10"/>
-      <c r="E4" s="20"/>
+      <c r="E4" s="21"/>
       <c r="F4" s="10" t="s">
         <v>88</v>
       </c>
@@ -2294,7 +2297,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,7 +2352,7 @@
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>104</v>
@@ -2379,14 +2382,14 @@
         <v>26</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2403,7 +2406,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2458,7 +2461,7 @@
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>93</v>
@@ -2553,7 +2556,7 @@
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>91</v>
@@ -2648,7 +2651,7 @@
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>90</v>
@@ -2743,7 +2746,7 @@
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>88</v>
@@ -3043,7 +3046,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>49</v>
@@ -3053,7 +3056,7 @@
         <v>83</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -3065,6 +3068,509 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480C7C36-EF9F-46B8-80F6-5D4D52F85692}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3FB4604-FCFA-4274-9E78-5F666179F7D7}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42A9E2B-D786-462A-BA24-F2C871073DDA}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="9" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E4:E6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909ACE9C-15FB-426D-9901-31B8FE57EC5F}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -3142,7 +3648,7 @@
         <v>50</v>
       </c>
       <c r="D4" s="10"/>
-      <c r="E4" s="20"/>
+      <c r="E4" s="21"/>
       <c r="F4" s="10" t="s">
         <v>103</v>
       </c>
@@ -3172,505 +3678,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480C7C36-EF9F-46B8-80F6-5D4D52F85692}">
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3FB4604-FCFA-4274-9E78-5F666179F7D7}">
-  <dimension ref="A1:F12"/>
-  <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D12" s="12"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42A9E2B-D786-462A-BA24-F2C871073DDA}">
-  <dimension ref="A1:F12"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="9" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="10" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D12" s="12"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E4:E6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Create new folder name "Image"
Image is folder hold all import images in this project. It is divided
into many small folders fot easier management.
</commit_message>
<xml_diff>
--- a/Document/Final-Design-Database.xlsx
+++ b/Document/Final-Design-Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PTIT-BookStore-Website-Project\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PTIT-Bookstore-E-commerce-Website\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F31EA4-A6E6-445C-8FED-07CBA331B5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87AADAA-3E3E-4E63-8E3F-C43E71F2847A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QUICKLOOK" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="175">
   <si>
     <t>SatisfyProduct</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Author</t>
   </si>
   <si>
-    <t>FullName</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -364,9 +361,6 @@
     <t>varchar(50)</t>
   </si>
   <si>
-    <t>Họ và tên khách hàng</t>
-  </si>
-  <si>
     <t>Địa chỉ email khách hàng</t>
   </si>
   <si>
@@ -409,9 +403,6 @@
     <t>PK (FK, NOT NULL)</t>
   </si>
   <si>
-    <t>NOT NULL, Default = now()</t>
-  </si>
-  <si>
     <t>Mã đơn đặt hàng</t>
   </si>
   <si>
@@ -460,9 +451,6 @@
     <t>Phải từ 18 tuổi trở lên</t>
   </si>
   <si>
-    <t>Họ và tên nhân viên</t>
-  </si>
-  <si>
     <t>Địa chỉ email nhân viên</t>
   </si>
   <si>
@@ -545,6 +533,36 @@
   </si>
   <si>
     <t>PromotionName</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>nvarchar(40)</t>
+  </si>
+  <si>
+    <t>nvarchar(10)</t>
+  </si>
+  <si>
+    <t>Tên khách hàng</t>
+  </si>
+  <si>
+    <t>Họ khách hàng</t>
+  </si>
+  <si>
+    <t>Tên nhân viên</t>
+  </si>
+  <si>
+    <t>Họ nhân viên</t>
+  </si>
+  <si>
+    <t>NOT NULL, Default = GETDATE()</t>
+  </si>
+  <si>
+    <t>nvarchar(200)</t>
   </si>
 </sst>
 </file>
@@ -717,7 +735,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -736,6 +754,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1037,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,7 +1079,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3" t="s">
@@ -1072,11 +1091,11 @@
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J1" s="2"/>
       <c r="L1" s="2"/>
@@ -1091,19 +1110,19 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J2" s="2"/>
       <c r="L2" s="14" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -1112,7 +1131,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="4" t="s">
@@ -1124,7 +1143,7 @@
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J3" s="2"/>
       <c r="L3" s="3" t="s">
@@ -1139,24 +1158,24 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="5" t="s">
-        <v>11</v>
+        <v>166</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J4" s="2"/>
       <c r="L4" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
@@ -1165,11 +1184,11 @@
       <c r="D5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="5" t="s">
-        <v>16</v>
+        <v>165</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J5" s="2"/>
       <c r="L5" s="15" t="s">
@@ -1178,23 +1197,23 @@
     </row>
     <row r="6" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -1202,19 +1221,19 @@
     </row>
     <row r="7" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H7" s="2"/>
       <c r="J7" s="2"/>
@@ -1223,30 +1242,30 @@
     </row>
     <row r="8" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
@@ -1254,12 +1273,15 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F9" s="2"/>
+      <c r="G9" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -1269,19 +1291,16 @@
     </row>
     <row r="10" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="4" t="s">
         <v>4</v>
@@ -1294,71 +1313,71 @@
     </row>
     <row r="11" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="4" t="s">
-        <v>121</v>
+      <c r="G11" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="5" t="s">
-        <v>16</v>
+      <c r="G12" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L13" s="17" t="s">
         <v>4</v>
@@ -1366,57 +1385,57 @@
     </row>
     <row r="14" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J14" s="2"/>
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="5" t="s">
-        <v>59</v>
+        <v>166</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J15" s="2"/>
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="4" t="s">
@@ -1424,7 +1443,7 @@
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="5" t="s">
-        <v>61</v>
+        <v>165</v>
       </c>
       <c r="H16" s="2"/>
       <c r="J16" s="2"/>
@@ -1432,19 +1451,19 @@
     </row>
     <row r="17" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" s="2"/>
-      <c r="G17" s="8" t="s">
-        <v>14</v>
+      <c r="G17" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="H17" s="2"/>
       <c r="J17" s="2"/>
@@ -1452,19 +1471,19 @@
     </row>
     <row r="18" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="5" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="H18" s="2"/>
       <c r="J18" s="2"/>
@@ -1472,16 +1491,16 @@
     </row>
     <row r="19" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="5" t="s">
-        <v>19</v>
+      <c r="G19" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="H19" s="2"/>
       <c r="J19" s="2"/>
@@ -1490,12 +1509,12 @@
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H20" s="2"/>
       <c r="J20" s="2"/>
@@ -1506,7 +1525,7 @@
       <c r="D21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H21" s="2"/>
       <c r="J21" s="2"/>
@@ -1516,7 +1535,7 @@
       <c r="D22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="5" t="s">
-        <v>164</v>
+        <v>20</v>
       </c>
       <c r="H22" s="2"/>
       <c r="J22" s="2"/>
@@ -1525,6 +1544,9 @@
       <c r="B23" s="2"/>
       <c r="D23" s="2"/>
       <c r="F23" s="2"/>
+      <c r="G23" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="H23" s="2"/>
       <c r="J23" s="2"/>
       <c r="L23" s="2"/>
@@ -1534,6 +1556,9 @@
       <c r="B24" s="2"/>
       <c r="D24" s="2"/>
       <c r="F24" s="2"/>
+      <c r="G24" s="5" t="s">
+        <v>160</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="J24" s="2"/>
       <c r="L24" s="2"/>
@@ -1640,33 +1665,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="A1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1674,17 +1699,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1692,17 +1717,17 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1715,10 +1740,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD6ACA7-C054-4542-B51D-AF4DF0646942}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,33 +1757,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="A1" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1766,17 +1791,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1784,17 +1809,17 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1805,14 +1830,14 @@
         <v>9</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1820,37 +1845,39 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>166</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="F6" s="10" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="D7" s="10"/>
+      <c r="B7" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="E7" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1858,17 +1885,17 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>162</v>
+        <v>58</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1876,17 +1903,17 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>158</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>48</v>
+        <v>131</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1894,17 +1921,17 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1912,17 +1939,17 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1930,17 +1957,17 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>112</v>
+        <v>49</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1948,17 +1975,17 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1966,17 +1993,35 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>164</v>
+        <v>21</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>135</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1992,7 +2037,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2001,39 +2046,39 @@
     <col min="2" max="2" width="24.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="A1" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2041,17 +2086,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2059,17 +2104,17 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2077,17 +2122,17 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2095,17 +2140,17 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>123</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2113,17 +2158,17 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2131,17 +2176,17 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2149,19 +2194,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="F9" s="10" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2191,33 +2236,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="A1" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2225,17 +2270,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="E3" s="19" t="s">
-        <v>122</v>
+      <c r="E3" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2246,12 +2291,12 @@
         <v>4</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="10"/>
-      <c r="E4" s="21"/>
+      <c r="E4" s="22"/>
       <c r="F4" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2259,17 +2304,17 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2277,17 +2322,17 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2318,33 +2363,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="A1" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2352,17 +2397,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="E3" s="22" t="s">
-        <v>155</v>
+      <c r="E3" s="23" t="s">
+        <v>151</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2373,12 +2418,12 @@
         <v>4</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="23"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2386,17 +2431,17 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="13" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2428,33 +2473,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2462,17 +2507,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2480,19 +2525,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2523,33 +2568,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2557,17 +2602,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2575,19 +2620,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2618,33 +2663,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2655,14 +2700,14 @@
         <v>8</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2670,19 +2715,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2697,8 +2742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D0EF8C-9832-4464-BAB8-BACE24741B9F}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:F20"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2713,33 +2758,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="A1" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2750,14 +2795,14 @@
         <v>4</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2768,13 +2813,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>38</v>
+        <v>174</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2785,14 +2830,14 @@
         <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2800,17 +2845,17 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2818,17 +2863,17 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2836,17 +2881,17 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2854,17 +2899,17 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2872,17 +2917,17 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2890,17 +2935,17 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2908,17 +2953,17 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2926,17 +2971,17 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2944,19 +2989,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D14" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="F14" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2964,17 +3009,17 @@
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2982,17 +3027,17 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3000,17 +3045,17 @@
         <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3018,17 +3063,17 @@
         <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3036,17 +3081,17 @@
         <v>17</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3054,17 +3099,17 @@
         <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -3095,33 +3140,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="A1" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3129,17 +3174,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3147,19 +3192,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="F4" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3167,17 +3212,17 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3185,17 +3230,17 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3203,17 +3248,17 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3221,17 +3266,17 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -3247,7 +3292,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:F9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3262,33 +3307,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="A1" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3296,17 +3341,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3317,14 +3362,14 @@
         <v>9</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3332,37 +3377,39 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>166</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>38</v>
+        <v>167</v>
       </c>
       <c r="D5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="F5" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="10"/>
+      <c r="B6" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="E6" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>109</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3370,17 +3417,17 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>48</v>
+        <v>106</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3388,17 +3435,17 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3406,17 +3453,35 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>110</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3449,33 +3514,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="A1" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3483,17 +3548,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3501,17 +3566,17 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="10"/>
-      <c r="E4" s="19" t="s">
-        <v>46</v>
+      <c r="E4" s="20" t="s">
+        <v>45</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3519,15 +3584,15 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D5" s="10"/>
-      <c r="E5" s="20"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="10" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3535,17 +3600,17 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="21"/>
+        <v>41</v>
+      </c>
+      <c r="E6" s="22"/>
       <c r="F6" s="10" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3553,17 +3618,17 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3598,33 +3663,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3632,17 +3697,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="E3" s="19" t="s">
-        <v>122</v>
+      <c r="E3" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3653,12 +3718,12 @@
         <v>4</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="10"/>
-      <c r="E4" s="21"/>
+      <c r="E4" s="22"/>
       <c r="F4" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3666,17 +3731,17 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Encrypt pwd & Regenerate script
</commit_message>
<xml_diff>
--- a/Document/Final-Design-Database.xlsx
+++ b/Document/Final-Design-Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PTIT-Bookstore-E-commerce-Website\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87AADAA-3E3E-4E63-8E3F-C43E71F2847A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804F8ECB-03E4-472E-945F-B910F478EB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QUICKLOOK" sheetId="1" r:id="rId1"/>
@@ -346,9 +346,6 @@
     <t>Mã khách hàng</t>
   </si>
   <si>
-    <t>varchar(128)</t>
-  </si>
-  <si>
     <t>Lưu pwd đã được mã hóa</t>
   </si>
   <si>
@@ -563,6 +560,9 @@
   </si>
   <si>
     <t>nvarchar(200)</t>
+  </si>
+  <si>
+    <t>char(32)</t>
   </si>
 </sst>
 </file>
@@ -1095,7 +1095,7 @@
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J1" s="2"/>
       <c r="L1" s="2"/>
@@ -1118,11 +1118,11 @@
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J2" s="2"/>
       <c r="L2" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -1131,7 +1131,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="4" t="s">
@@ -1162,7 +1162,7 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="5" t="s">
@@ -1184,7 +1184,7 @@
       <c r="D5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="5" t="s">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="4" t="s">
@@ -1247,7 +1247,7 @@
       <c r="B8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="5" t="s">
@@ -1317,7 +1317,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="5" t="s">
@@ -1339,7 +1339,7 @@
     </row>
     <row r="12" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B12" s="2"/>
       <c r="D12" s="2"/>
@@ -1348,7 +1348,7 @@
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -1412,7 +1412,7 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="4" t="s">
@@ -1420,7 +1420,7 @@
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="5" t="s">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="4" t="s">
@@ -1443,7 +1443,7 @@
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H16" s="2"/>
       <c r="J16" s="2"/>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="19" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="5" t="s">
@@ -1557,7 +1557,7 @@
       <c r="D24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H24" s="2"/>
       <c r="J24" s="2"/>
@@ -1706,10 +1706,10 @@
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1720,14 +1720,14 @@
         <v>63</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
         <v>42</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1742,8 +1742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD6ACA7-C054-4542-B51D-AF4DF0646942}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1791,17 +1791,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1812,14 +1812,14 @@
         <v>15</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
         <v>45</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1830,14 +1830,14 @@
         <v>9</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
         <v>42</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1845,7 +1845,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>37</v>
@@ -1857,7 +1857,7 @@
         <v>42</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1865,10 +1865,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>41</v>
@@ -1877,7 +1877,7 @@
         <v>42</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1888,14 +1888,14 @@
         <v>58</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
         <v>45</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1903,17 +1903,17 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10" t="s">
         <v>45</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1931,7 +1931,7 @@
         <v>80</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1949,7 +1949,7 @@
         <v>80</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1967,7 +1967,7 @@
         <v>42</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -1978,14 +1978,14 @@
         <v>20</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10" t="s">
         <v>42</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2003,7 +2003,7 @@
         <v>42</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2011,7 +2011,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>47</v>
@@ -2021,7 +2021,7 @@
         <v>80</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2093,10 +2093,10 @@
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2104,7 +2104,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>38</v>
@@ -2114,7 +2114,7 @@
         <v>43</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2132,7 +2132,7 @@
         <v>43</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2147,10 +2147,10 @@
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2158,7 +2158,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>39</v>
@@ -2168,7 +2168,7 @@
         <v>43</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2183,10 +2183,10 @@
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2206,7 +2206,7 @@
         <v>42</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2277,10 +2277,10 @@
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>120</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2314,7 +2314,7 @@
         <v>44</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2329,10 +2329,10 @@
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2404,7 +2404,7 @@
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>101</v>
@@ -2434,14 +2434,14 @@
         <v>24</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2514,7 +2514,7 @@
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>90</v>
@@ -2525,7 +2525,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>37</v>
@@ -2609,7 +2609,7 @@
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>88</v>
@@ -2620,7 +2620,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>37</v>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>87</v>
@@ -2715,7 +2715,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>37</v>
@@ -2742,8 +2742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D0EF8C-9832-4464-BAB8-BACE24741B9F}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2799,7 +2799,7 @@
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>85</v>
@@ -2813,7 +2813,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>42</v>
@@ -2942,7 +2942,7 @@
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>92</v>
@@ -2953,7 +2953,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>75</v>
@@ -3099,7 +3099,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>47</v>
@@ -3109,7 +3109,7 @@
         <v>80</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -3181,10 +3181,10 @@
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3192,10 +3192,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>41</v>
@@ -3204,7 +3204,7 @@
         <v>42</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3222,7 +3222,7 @@
         <v>42</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3240,7 +3240,7 @@
         <v>42</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3255,10 +3255,10 @@
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3266,17 +3266,17 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>75</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -3292,7 +3292,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3348,7 +3348,7 @@
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>101</v>
@@ -3362,14 +3362,14 @@
         <v>9</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
         <v>42</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3377,10 +3377,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>166</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>167</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>41</v>
@@ -3389,7 +3389,7 @@
         <v>42</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3397,10 +3397,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>41</v>
@@ -3409,7 +3409,7 @@
         <v>42</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3420,14 +3420,14 @@
         <v>15</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
         <v>45</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3445,7 +3445,7 @@
         <v>80</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3463,7 +3463,7 @@
         <v>42</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3481,7 +3481,7 @@
         <v>42</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3515,7 +3515,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -3548,17 +3548,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>38</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3587,12 +3587,12 @@
         <v>68</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="21"/>
       <c r="F5" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3603,14 +3603,14 @@
         <v>69</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>41</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3628,7 +3628,7 @@
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3704,7 +3704,7 @@
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Edit data type for encrypting
- Edit data types of UserID, StaffID and both pwd in SQL Server
- Edit them in Excel and Word report too.
</commit_message>
<xml_diff>
--- a/Document/Final-Design-Database.xlsx
+++ b/Document/Final-Design-Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PTIT-Bookstore-E-commerce-Website\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804F8ECB-03E4-472E-945F-B910F478EB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724D7DB6-AE41-4DB8-B38D-C370610192EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QUICKLOOK" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="176">
   <si>
     <t>SatisfyProduct</t>
   </si>
@@ -562,7 +562,10 @@
     <t>nvarchar(200)</t>
   </si>
   <si>
-    <t>char(32)</t>
+    <t>char(36)</t>
+  </si>
+  <si>
+    <t>char(60)</t>
   </si>
 </sst>
 </file>
@@ -1742,7 +1745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD6ACA7-C054-4542-B51D-AF4DF0646942}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1794,7 +1797,7 @@
         <v>118</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>39</v>
+        <v>174</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
@@ -1830,7 +1833,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
@@ -3291,8 +3294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3FB4604-FCFA-4274-9E78-5F666179F7D7}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3344,7 +3347,7 @@
         <v>98</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>39</v>
+        <v>174</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
@@ -3362,7 +3365,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">

</xml_diff>

<commit_message>
Regenerate script + Write report for end-of-term
</commit_message>
<xml_diff>
--- a/Document/Final-Design-Database.xlsx
+++ b/Document/Final-Design-Database.xlsx
@@ -8,25 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PTIT-Bookstore-E-commerce-Website\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724D7DB6-AE41-4DB8-B38D-C370610192EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A3C64D-CA42-46BE-9A20-299AC1065E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="QUICKLOOK" sheetId="1" r:id="rId1"/>
-    <sheet name="PUBLISHER" sheetId="16" r:id="rId2"/>
-    <sheet name="AUTHOR" sheetId="15" r:id="rId3"/>
-    <sheet name="CATEGORY" sheetId="14" r:id="rId4"/>
-    <sheet name="BOOK" sheetId="2" r:id="rId5"/>
-    <sheet name="PROMOTION" sheetId="20" r:id="rId6"/>
-    <sheet name="USERACCOUNT" sheetId="18" r:id="rId7"/>
-    <sheet name="DELIVERYINFORMATION" sheetId="24" r:id="rId8"/>
-    <sheet name="CART" sheetId="17" r:id="rId9"/>
-    <sheet name="MASTERROLE" sheetId="26" r:id="rId10"/>
-    <sheet name="STAFFACCOUNT" sheetId="23" r:id="rId11"/>
-    <sheet name="ORDER" sheetId="21" r:id="rId12"/>
-    <sheet name="ORDERDETAIL" sheetId="22" r:id="rId13"/>
-    <sheet name="RATING" sheetId="25" r:id="rId14"/>
+    <sheet name="PUBLISHER" sheetId="16" r:id="rId1"/>
+    <sheet name="AUTHOR" sheetId="15" r:id="rId2"/>
+    <sheet name="CATEGORY" sheetId="14" r:id="rId3"/>
+    <sheet name="BOOK" sheetId="2" r:id="rId4"/>
+    <sheet name="PROMOTION" sheetId="20" r:id="rId5"/>
+    <sheet name="USERACCOUNT" sheetId="18" r:id="rId6"/>
+    <sheet name="CART" sheetId="17" r:id="rId7"/>
+    <sheet name="ROLE" sheetId="26" r:id="rId8"/>
+    <sheet name="STAFFACCOUNT" sheetId="23" r:id="rId9"/>
+    <sheet name="ORDER" sheetId="21" r:id="rId10"/>
+    <sheet name="ORDERDETAIL" sheetId="22" r:id="rId11"/>
+    <sheet name="SATISFYPRODUCT" sheetId="28" r:id="rId12"/>
+    <sheet name="HISTORYTable" sheetId="29" r:id="rId13"/>
+    <sheet name="(OLD)QUICKLOOK" sheetId="1" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="220">
   <si>
     <t>SatisfyProduct</t>
   </si>
@@ -238,9 +238,6 @@
     <t>Cover</t>
   </si>
   <si>
-    <t>IsDiscount</t>
-  </si>
-  <si>
     <t>RecipientName</t>
   </si>
   <si>
@@ -319,15 +316,9 @@
     <t>Giá gốc (không tính giảm giá)</t>
   </si>
   <si>
-    <t>Phần trăm giảm giá nếu IsDiscount = 1</t>
-  </si>
-  <si>
     <t>Tên thể loại</t>
   </si>
   <si>
-    <t>nvarchar(20)</t>
-  </si>
-  <si>
     <t>Tên tác giả</t>
   </si>
   <si>
@@ -346,27 +337,9 @@
     <t>Mã khách hàng</t>
   </si>
   <si>
-    <t>Lưu pwd đã được mã hóa</t>
-  </si>
-  <si>
-    <t>0 là nam, 1 là nữ</t>
-  </si>
-  <si>
-    <t>Phải trên 18 tuổi</t>
-  </si>
-  <si>
     <t>varchar(50)</t>
   </si>
   <si>
-    <t>Địa chỉ email khách hàng</t>
-  </si>
-  <si>
-    <t>Ảnh đại diện</t>
-  </si>
-  <si>
-    <t>DiscountPercent</t>
-  </si>
-  <si>
     <t>nvarchar(100)</t>
   </si>
   <si>
@@ -403,18 +376,6 @@
     <t>Mã đơn đặt hàng</t>
   </si>
   <si>
-    <t>Mã người nhận hàng</t>
-  </si>
-  <si>
-    <t>Ngày tạo đơn hàng</t>
-  </si>
-  <si>
-    <t>Mã nhân viên</t>
-  </si>
-  <si>
-    <t>Tổng tiền (không tính ship)</t>
-  </si>
-  <si>
     <t>Trạng thái đơn hàng</t>
   </si>
   <si>
@@ -433,33 +394,12 @@
     <t>char(10)</t>
   </si>
   <si>
-    <t>0 là đang làm, 1 là đã nghỉ</t>
-  </si>
-  <si>
     <t>0 là vẫn kinh doanh, 1 là không còn kinh doanh</t>
   </si>
   <si>
     <t>PK</t>
   </si>
   <si>
-    <t>0 là staff, 1 là admin</t>
-  </si>
-  <si>
-    <t>Phải từ 18 tuổi trở lên</t>
-  </si>
-  <si>
-    <t>Địa chỉ email nhân viên</t>
-  </si>
-  <si>
-    <t>CCCD nhân viên</t>
-  </si>
-  <si>
-    <t>SĐT nhân viên</t>
-  </si>
-  <si>
-    <t>Địa chỉ nhà nhân viên</t>
-  </si>
-  <si>
     <t>PK, ID tăng dần</t>
   </si>
   <si>
@@ -475,45 +415,15 @@
     <t>isDiscount</t>
   </si>
   <si>
-    <t>tinyint</t>
-  </si>
-  <si>
-    <t>Mã thông tin nhận hàng</t>
-  </si>
-  <si>
     <t>Địa chỉ nhận hàng</t>
   </si>
   <si>
-    <t>SĐT người nhận hàng</t>
-  </si>
-  <si>
-    <t>Tên người nhận hàng</t>
-  </si>
-  <si>
-    <t>PK(FK, NOT NULL)</t>
-  </si>
-  <si>
-    <t>Số sao từ 1 đến 5</t>
-  </si>
-  <si>
-    <t>NOT NULL, giá trị 1-5</t>
-  </si>
-  <si>
-    <t>char(5)</t>
-  </si>
-  <si>
-    <t>PK, giá trị 0 hoặc 1, Default = 0</t>
-  </si>
-  <si>
     <t>Tên quyền</t>
   </si>
   <si>
     <t>Ý tưởng thông minh</t>
   </si>
   <si>
-    <t>Phone</t>
-  </si>
-  <si>
     <t>IsDiscontinued</t>
   </si>
   <si>
@@ -538,34 +448,256 @@
     <t>LastName</t>
   </si>
   <si>
-    <t>nvarchar(40)</t>
-  </si>
-  <si>
-    <t>nvarchar(10)</t>
-  </si>
-  <si>
-    <t>Tên khách hàng</t>
-  </si>
-  <si>
-    <t>Họ khách hàng</t>
-  </si>
-  <si>
-    <t>Tên nhân viên</t>
-  </si>
-  <si>
-    <t>Họ nhân viên</t>
-  </si>
-  <si>
     <t>NOT NULL, Default = GETDATE()</t>
   </si>
   <si>
     <t>nvarchar(200)</t>
   </si>
   <si>
-    <t>char(36)</t>
-  </si>
-  <si>
     <t>char(60)</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>Tên đăng nhập</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>full_name</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>birthday</t>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
+  <si>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>nvarchar(60)</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Địa chỉ email</t>
+  </si>
+  <si>
+    <t>Họ và tên</t>
+  </si>
+  <si>
+    <t>Giới tính</t>
+  </si>
+  <si>
+    <t>Ngày sinh</t>
+  </si>
+  <si>
+    <t>Mật khẩu đã được mã hóa</t>
+  </si>
+  <si>
+    <t>Giới tính (0: nam, 1:nữ)</t>
+  </si>
+  <si>
+    <t>Trạng thái tài khoản                      (0 là chưa kích hoạt, 1 là đã kích hoạt)</t>
+  </si>
+  <si>
+    <t>varchar(36)</t>
+  </si>
+  <si>
+    <t>staff_id</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>id_card</t>
+  </si>
+  <si>
+    <t>role_id</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>is_quit</t>
+  </si>
+  <si>
+    <t>varchar(5)</t>
+  </si>
+  <si>
+    <t>Số điện thoại</t>
+  </si>
+  <si>
+    <t>Mã định danh</t>
+  </si>
+  <si>
+    <t>Mã quyền</t>
+  </si>
+  <si>
+    <t>Địa chỉ</t>
+  </si>
+  <si>
+    <t>Mật khẩu đã mã hóa</t>
+  </si>
+  <si>
+    <t>Trạng thái nghỉ việc                      (0 là đang làm, 1 là đã nghỉ việc)</t>
+  </si>
+  <si>
+    <t>history_id</t>
+  </si>
+  <si>
+    <t>isbn</t>
+  </si>
+  <si>
+    <t>Mã lịch sử</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>role_name</t>
+  </si>
+  <si>
+    <t>publisher_id</t>
+  </si>
+  <si>
+    <t>publisher_name</t>
+  </si>
+  <si>
+    <t>promotion_id</t>
+  </si>
+  <si>
+    <t>promotion_name</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>discount_percent</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>order_detail_id</t>
+  </si>
+  <si>
+    <t>order_id</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>bigint</t>
+  </si>
+  <si>
+    <t>Mã chi tiết đơn đặt hàng</t>
+  </si>
+  <si>
+    <t>order_date</t>
+  </si>
+  <si>
+    <t>receiver</t>
+  </si>
+  <si>
+    <t>payment_method</t>
+  </si>
+  <si>
+    <t>order_status</t>
+  </si>
+  <si>
+    <t>total_price</t>
+  </si>
+  <si>
+    <t>Ngày đặt</t>
+  </si>
+  <si>
+    <t>Tên người nhận</t>
+  </si>
+  <si>
+    <t>Phương thức thanh toán</t>
+  </si>
+  <si>
+    <t>Tổng tiền</t>
+  </si>
+  <si>
+    <t>request_time</t>
+  </si>
+  <si>
+    <t>session_id</t>
+  </si>
+  <si>
+    <t>Thời gian request</t>
+  </si>
+  <si>
+    <t>Mã session</t>
+  </si>
+  <si>
+    <t>category_id</t>
+  </si>
+  <si>
+    <t>category_name</t>
+  </si>
+  <si>
+    <t>cart_id</t>
+  </si>
+  <si>
+    <t>Mã giỏ hàng</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>author_id</t>
+  </si>
+  <si>
+    <t>year_of_publication</t>
+  </si>
+  <si>
+    <t>cover</t>
+  </si>
+  <si>
+    <t>is_discount</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>url1</t>
+  </si>
+  <si>
+    <t>url2</t>
+  </si>
+  <si>
+    <t>url3</t>
+  </si>
+  <si>
+    <t>url4</t>
+  </si>
+  <si>
+    <t>url5</t>
+  </si>
+  <si>
+    <t>is_discontinued</t>
+  </si>
+  <si>
+    <t>Phần trăm giảm giá nếu is_discount = 1</t>
+  </si>
+  <si>
+    <t>author_name</t>
   </si>
 </sst>
 </file>
@@ -738,7 +870,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -752,7 +884,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -764,17 +895,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1056,11 +1192,711 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9932C816-0A00-45D4-8AE3-45E3F6116964}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE317E5-52A0-4284-95B8-DCBD3874C7B7}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>9</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B786C6-460B-4BC0-8724-D85868BC7020}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A7" sqref="A1:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="22">
+        <v>5</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2942826D-B6D6-44D2-A68B-89D95E1FDE61}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E3:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DAB3F10-9457-40BD-ADC8-782F5EF4CA2D}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="22">
+        <v>5</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,7 +1934,7 @@
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="1" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="J1" s="2"/>
       <c r="L1" s="2"/>
@@ -1113,19 +1949,19 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="4" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="J2" s="2"/>
-      <c r="L2" s="14" t="s">
-        <v>156</v>
+      <c r="L2" s="13" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -1134,7 +1970,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="5" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="4" t="s">
@@ -1146,7 +1982,7 @@
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J3" s="2"/>
       <c r="L3" s="3" t="s">
@@ -1165,14 +2001,14 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="5" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J4" s="2"/>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="14" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1187,14 +2023,14 @@
       <c r="D5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="5" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J5" s="2"/>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="14" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1208,7 +2044,7 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="5" t="s">
@@ -1216,11 +2052,11 @@
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="16"/>
+      <c r="L6" s="15"/>
     </row>
     <row r="7" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -1228,11 +2064,11 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="5" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="5" t="s">
@@ -1241,7 +2077,7 @@
       <c r="H7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="16"/>
+      <c r="L7" s="15"/>
     </row>
     <row r="8" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -1250,7 +2086,7 @@
       <c r="B8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="5" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="5" t="s">
@@ -1276,7 +2112,7 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="5" t="s">
@@ -1284,11 +2120,11 @@
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="15" t="s">
+      <c r="L9" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1301,7 +2137,7 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F10" s="2"/>
       <c r="H10" s="2"/>
@@ -1310,7 +2146,7 @@
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="17" t="s">
+      <c r="L10" s="16" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1320,11 +2156,11 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="5" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="3" t="s">
@@ -1336,13 +2172,13 @@
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="17" t="s">
+      <c r="L11" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="B12" s="2"/>
       <c r="D12" s="2"/>
@@ -1351,13 +2187,13 @@
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="4" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="17" t="s">
+      <c r="L12" s="16" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1382,7 +2218,7 @@
       <c r="K13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="L13" s="17" t="s">
+      <c r="L13" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1415,7 +2251,7 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="8" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="4" t="s">
@@ -1423,7 +2259,7 @@
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="5" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="5" t="s">
@@ -1438,7 +2274,7 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="5" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="4" t="s">
@@ -1446,7 +2282,7 @@
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="5" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="H16" s="2"/>
       <c r="J16" s="2"/>
@@ -1458,7 +2294,7 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="5" t="s">
@@ -1494,7 +2330,7 @@
     </row>
     <row r="19" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="5" t="s">
@@ -1560,7 +2396,7 @@
       <c r="D24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="5" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="H24" s="2"/>
       <c r="J24" s="2"/>
@@ -1648,915 +2484,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75EA8E3B-A636-4F2F-9E57-AF78DE5C1A08}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="9"/>
-    <col min="2" max="2" width="11.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="9"/>
-    <col min="4" max="4" width="11" style="9" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD6ACA7-C054-4542-B51D-AF4DF0646942}">
-  <dimension ref="A1:F15"/>
-  <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
-        <v>5</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>9</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>10</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>11</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
-        <v>12</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>13</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE317E5-52A0-4284-95B8-DCBD3874C7B7}">
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B786C6-460B-4BC0-8724-D85868BC7020}">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:F6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E3:E4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F846A4FA-0134-4117-B6D3-507C28FB8D47}">
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E3:E4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9932C816-0A00-45D4-8AE3-45E3F6116964}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0D6478-39EB-4578-96B5-12DCD2A33FB0}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2571,14 +2504,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -2605,17 +2538,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>50</v>
+        <v>207</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>39</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2623,7 +2556,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>161</v>
+        <v>219</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>37</v>
@@ -2635,7 +2568,7 @@
         <v>45</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2646,12 +2579,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B7C92A-D9C5-4920-8FD0-E3215FDA0CAD}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2666,14 +2599,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -2700,17 +2633,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>202</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>39</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2718,7 +2651,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>160</v>
+        <v>203</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>37</v>
@@ -2730,7 +2663,7 @@
         <v>45</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2741,12 +2674,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D0EF8C-9832-4464-BAB8-BACE24741B9F}">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2761,14 +2694,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -2795,17 +2728,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>171</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2813,16 +2746,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>6</v>
+        <v>206</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>173</v>
+        <v>137</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>42</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2830,7 +2763,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>8</v>
+        <v>202</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>39</v>
@@ -2840,7 +2773,7 @@
         <v>43</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2848,7 +2781,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>50</v>
+        <v>207</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>39</v>
@@ -2858,7 +2791,7 @@
         <v>43</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2866,17 +2799,17 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>208</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2884,7 +2817,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>14</v>
+        <v>175</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>39</v>
@@ -2894,7 +2827,7 @@
         <v>43</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2902,7 +2835,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>11</v>
+        <v>185</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>38</v>
@@ -2912,7 +2845,7 @@
         <v>44</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2920,17 +2853,17 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>65</v>
+        <v>209</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>47</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2938,17 +2871,17 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>16</v>
+        <v>186</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2956,17 +2889,17 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>108</v>
+        <v>181</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>93</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2974,17 +2907,17 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>66</v>
+        <v>210</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>47</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -2992,10 +2925,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>19</v>
+        <v>211</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>41</v>
@@ -3004,7 +2937,7 @@
         <v>42</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3012,17 +2945,17 @@
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>53</v>
+        <v>212</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10" t="s">
         <v>42</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3030,17 +2963,17 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>54</v>
+        <v>213</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10" t="s">
         <v>42</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3048,17 +2981,17 @@
         <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>55</v>
+        <v>214</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10" t="s">
         <v>42</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3066,17 +2999,17 @@
         <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>56</v>
+        <v>215</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10" t="s">
         <v>42</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3084,17 +3017,17 @@
         <v>17</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>57</v>
+        <v>216</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10" t="s">
         <v>42</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3102,17 +3035,17 @@
         <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>158</v>
+        <v>217</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>47</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -3123,12 +3056,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480C7C36-EF9F-46B8-80F6-5D4D52F85692}">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3143,14 +3076,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="A1" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -3177,17 +3110,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>70</v>
+        <v>177</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3195,10 +3128,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>41</v>
@@ -3207,7 +3140,7 @@
         <v>42</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3215,17 +3148,17 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>73</v>
+        <v>179</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>49</v>
+        <v>148</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
         <v>42</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3233,17 +3166,17 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>72</v>
+        <v>180</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>49</v>
+        <v>148</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
         <v>42</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3251,17 +3184,17 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3269,17 +3202,17 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>108</v>
+        <v>181</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -3290,12 +3223,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3FB4604-FCFA-4274-9E78-5F666179F7D7}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3310,14 +3243,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -3344,17 +3277,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>98</v>
+        <v>139</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3362,17 +3295,17 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>175</v>
+        <v>99</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3380,10 +3313,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>165</v>
+        <v>142</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>41</v>
@@ -3392,27 +3325,25 @@
         <v>42</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>164</v>
+      <c r="B6" s="5" t="s">
+        <v>143</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>41</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3420,17 +3351,17 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>15</v>
+        <v>144</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>106</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3438,57 +3369,39 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>17</v>
+        <v>145</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>47</v>
+        <v>138</v>
       </c>
       <c r="D8" s="10"/>
-      <c r="E8" s="10" t="s">
-        <v>80</v>
+      <c r="E8" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>18</v>
+        <v>146</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D12" s="12"/>
+        <v>79</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3498,160 +3411,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42A9E2B-D786-462A-BA24-F2C871073DDA}">
-  <dimension ref="A1:F12"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="9" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D12" s="12"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E4:E6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909ACE9C-15FB-426D-9901-31B8FE57EC5F}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:F5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3666,14 +3431,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -3700,33 +3465,35 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>39</v>
+        <v>204</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>187</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="10" t="s">
         <v>119</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>101</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
+      <c r="B4" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="D4" s="10"/>
-      <c r="E4" s="22"/>
+      <c r="E4" s="25" t="s">
+        <v>43</v>
+      </c>
       <c r="F4" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -3734,23 +3501,407 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>39</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75EA8E3B-A636-4F2F-9E57-AF78DE5C1A08}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="9"/>
+    <col min="2" max="2" width="11.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="9" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD6ACA7-C054-4542-B51D-AF4DF0646942}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection sqref="A1:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>99</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Write report for end-term + regenerate script
</commit_message>
<xml_diff>
--- a/Document/Final-Design-Database.xlsx
+++ b/Document/Final-Design-Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PTIT-Bookstore-E-commerce-Website\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A3C64D-CA42-46BE-9A20-299AC1065E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD6DB4F-0487-45FB-B10A-4D0CD0ADCC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PUBLISHER" sheetId="16" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="222">
   <si>
     <t>SatisfyProduct</t>
   </si>
@@ -698,6 +698,12 @@
   </si>
   <si>
     <t>author_name</t>
+  </si>
+  <si>
+    <t>cluster</t>
+  </si>
+  <si>
+    <t>Cụm</t>
   </si>
 </sst>
 </file>
@@ -870,7 +876,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -889,6 +895,18 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -897,20 +915,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1195,8 +1199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9932C816-0A00-45D4-8AE3-45E3F6116964}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,14 +1215,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1306,14 +1310,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1532,14 +1536,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1572,7 +1576,7 @@
         <v>187</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="19" t="s">
         <v>119</v>
       </c>
       <c r="F3" s="7" t="s">
@@ -1590,7 +1594,7 @@
         <v>187</v>
       </c>
       <c r="D4" s="10"/>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="19" t="s">
         <v>43</v>
       </c>
       <c r="F4" s="10" t="s">
@@ -1634,13 +1638,13 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
+      <c r="A7" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="7"/>
@@ -1664,7 +1668,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,14 +1679,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1715,7 +1719,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="23" t="s">
         <v>110</v>
       </c>
       <c r="F3" s="10" t="s">
@@ -1733,7 +1737,7 @@
         <v>48</v>
       </c>
       <c r="D4" s="10"/>
-      <c r="E4" s="20"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="10" t="s">
         <v>84</v>
       </c>
@@ -1752,7 +1756,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1764,14 +1768,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1804,7 +1808,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="19" t="s">
         <v>119</v>
       </c>
       <c r="F3" s="7" t="s">
@@ -1822,7 +1826,7 @@
         <v>99</v>
       </c>
       <c r="D4" s="10"/>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="19" t="s">
         <v>43</v>
       </c>
       <c r="F4" s="10" t="s">
@@ -1866,13 +1870,13 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
+      <c r="A7" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="10" t="s">
         <v>37</v>
       </c>
       <c r="D7" s="7"/>
@@ -2489,7 +2493,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2504,14 +2508,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -2584,7 +2588,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2599,14 +2603,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -2676,10 +2680,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D0EF8C-9832-4464-BAB8-BACE24741B9F}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2694,14 +2698,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -3035,16 +3039,32 @@
         <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10" t="s">
+      <c r="D21" s="10"/>
+      <c r="E21" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F21" s="10" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3076,14 +3096,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -3243,14 +3263,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -3396,7 +3416,7 @@
       <c r="E9" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="18" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3431,14 +3451,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -3489,7 +3509,7 @@
         <v>99</v>
       </c>
       <c r="D4" s="10"/>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="20" t="s">
         <v>43</v>
       </c>
       <c r="F4" s="10" t="s">
@@ -3507,7 +3527,7 @@
         <v>48</v>
       </c>
       <c r="D5" s="10"/>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="21" t="s">
         <v>43</v>
       </c>
       <c r="F5" s="10" t="s">
@@ -3560,14 +3580,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -3652,14 +3672,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -3877,7 +3897,7 @@
       <c r="E13" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="18" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3895,7 +3915,7 @@
       <c r="E14" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="18" t="s">
         <v>169</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Report end of term
</commit_message>
<xml_diff>
--- a/Document/Final-Design-Database.xlsx
+++ b/Document/Final-Design-Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PTIT-Bookstore-E-commerce-Website\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD6DB4F-0487-45FB-B10A-4D0CD0ADCC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4FB002-A01B-47A9-AAF4-098DAF3395A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PUBLISHER" sheetId="16" r:id="rId1"/>
@@ -22,11 +22,12 @@
     <sheet name="CART" sheetId="17" r:id="rId7"/>
     <sheet name="ROLE" sheetId="26" r:id="rId8"/>
     <sheet name="STAFFACCOUNT" sheetId="23" r:id="rId9"/>
-    <sheet name="ORDER" sheetId="21" r:id="rId10"/>
-    <sheet name="ORDERDETAIL" sheetId="22" r:id="rId11"/>
-    <sheet name="SATISFYPRODUCT" sheetId="28" r:id="rId12"/>
-    <sheet name="HISTORYTable" sheetId="29" r:id="rId13"/>
-    <sheet name="(OLD)QUICKLOOK" sheetId="1" r:id="rId14"/>
+    <sheet name="RATING" sheetId="30" r:id="rId10"/>
+    <sheet name="ORDER" sheetId="21" r:id="rId11"/>
+    <sheet name="ORDERDETAIL" sheetId="22" r:id="rId12"/>
+    <sheet name="SATISFYPRODUCT" sheetId="28" r:id="rId13"/>
+    <sheet name="HISTORYTable" sheetId="29" r:id="rId14"/>
+    <sheet name="(OLD)QUICKLOOK" sheetId="1" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="224">
   <si>
     <t>SatisfyProduct</t>
   </si>
@@ -704,6 +705,12 @@
   </si>
   <si>
     <t>Cụm</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>Mức độ đánh giá</t>
   </si>
 </sst>
 </file>
@@ -876,7 +883,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -915,6 +922,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1291,11 +1304,110 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000214BC-76E1-4A9F-ACFE-5426632629BA}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="26"/>
+      <c r="E4" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D3:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE317E5-52A0-4284-95B8-DCBD3874C7B7}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1517,7 +1629,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B786C6-460B-4BC0-8724-D85868BC7020}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -1663,7 +1775,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2942826D-B6D6-44D2-A68B-89D95E1FDE61}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -1751,7 +1863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DAB3F10-9457-40BD-ADC8-782F5EF4CA2D}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -1895,7 +2007,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L30"/>
   <sheetViews>
@@ -2682,7 +2794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D0EF8C-9832-4464-BAB8-BACE24741B9F}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -3658,7 +3770,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:F5"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>